<commit_message>
Fix Date input problem
</commit_message>
<xml_diff>
--- a/Endpoints.xlsx
+++ b/Endpoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="12270"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="27795" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>/bookings</t>
   </si>
   <si>
-    <t>/bookings/{userId}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Status: 200
 Body:bookings List </t>
   </si>
@@ -153,6 +150,10 @@
   </si>
   <si>
     <t>/rooms/{id}</t>
+  </si>
+  <si>
+    <t>/bookings/
+user/{userId}</t>
   </si>
 </sst>
 </file>
@@ -605,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,42 +744,42 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -831,7 +832,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>10</v>
@@ -844,20 +845,20 @@
       <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>28</v>
+      <c r="B16" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -868,16 +869,16 @@
         <v>27</v>
       </c>
       <c r="C17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -890,7 +891,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -903,19 +904,19 @@
         <v>6</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix project setup. Add frontend
</commit_message>
<xml_diff>
--- a/Endpoints.xlsx
+++ b/Endpoints.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="27795" windowHeight="12150"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21825" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0" refMode="R1C1"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -594,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>